<commit_message>
Actualización 25 de febrero
</commit_message>
<xml_diff>
--- a/data_1708813067.xlsx
+++ b/data_1708813067.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jguallasamin/Desktop/Tesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E816ED18-5BE7-4F44-8F80-60CAC1FED14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4D7D2A-DA08-7842-BFF8-F205E3193574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,6 +262,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -300,10 +303,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +612,7 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -662,7 +665,7 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>11973785.1425696</v>
       </c>
       <c r="G2" t="s">
@@ -691,7 +694,7 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>12435932.463685</v>
       </c>
       <c r="G3" t="s">
@@ -720,7 +723,7 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>13192815.962079501</v>
       </c>
       <c r="G4" t="s">
@@ -749,7 +752,7 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>14555506.385736899</v>
       </c>
       <c r="G5" t="s">
@@ -778,7 +781,7 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>12757885.0546245</v>
       </c>
       <c r="G6" t="s">
@@ -807,7 +810,7 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>13167470.5829581</v>
       </c>
       <c r="G7" t="s">
@@ -836,7 +839,7 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>13455244.3160867</v>
       </c>
       <c r="G8" t="s">
@@ -865,7 +868,7 @@
       <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>14971349.2821417</v>
       </c>
       <c r="G9" t="s">
@@ -894,7 +897,7 @@
       <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>13314494.7734983</v>
       </c>
       <c r="G10" t="s">
@@ -923,7 +926,7 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>13815663.826254399</v>
       </c>
       <c r="G11" t="s">
@@ -952,7 +955,7 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>14177884.1575618</v>
       </c>
       <c r="G12" t="s">
@@ -981,7 +984,7 @@
       <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>15722422.909221999</v>
       </c>
       <c r="G13" t="s">
@@ -1010,7 +1013,7 @@
       <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>13903568.5575813</v>
       </c>
       <c r="G14" t="s">
@@ -1039,7 +1042,7 @@
       <c r="E15" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>13983215.3792329</v>
       </c>
       <c r="G15" t="s">
@@ -1068,7 +1071,7 @@
       <c r="E16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>14456706.330015</v>
       </c>
       <c r="G16" t="s">
@@ -1097,7 +1100,7 @@
       <c r="E17" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>16332019.777084799</v>
       </c>
       <c r="G17" t="s">
@@ -1126,7 +1129,7 @@
       <c r="E18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>14557302.5409599</v>
       </c>
       <c r="G18" t="s">
@@ -1155,7 +1158,7 @@
       <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>15036627.7095329</v>
       </c>
       <c r="G19" t="s">
@@ -1184,7 +1187,7 @@
       <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>15584558.4624754</v>
       </c>
       <c r="G20" t="s">
@@ -1213,7 +1216,7 @@
       <c r="E21" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <v>17505965.113824401</v>
       </c>
       <c r="G21" t="s">
@@ -1242,7 +1245,7 @@
       <c r="E22" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="3">
         <v>15482339.440911399</v>
       </c>
       <c r="G22" t="s">
@@ -1271,7 +1274,7 @@
       <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>15996967.900641801</v>
       </c>
       <c r="G23" t="s">
@@ -1300,7 +1303,7 @@
       <c r="E24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="3">
         <v>16340891.0951041</v>
       </c>
       <c r="G24" t="s">
@@ -1329,7 +1332,7 @@
       <c r="E25" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>18248351.597750999</v>
       </c>
       <c r="G25" t="s">
@@ -1358,7 +1361,7 @@
       <c r="E26" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>16174029.116040099</v>
       </c>
       <c r="G26" t="s">
@@ -1387,7 +1390,7 @@
       <c r="E27" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="3">
         <v>16669236.674202099</v>
       </c>
       <c r="G27" t="s">
@@ -1416,7 +1419,7 @@
       <c r="E28" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="3">
         <v>17236054.458573502</v>
       </c>
       <c r="G28" t="s">
@@ -1445,7 +1448,7 @@
       <c r="E29" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
         <v>18857353.619024601</v>
       </c>
       <c r="G29" t="s">
@@ -1474,7 +1477,7 @@
       <c r="E30" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="3">
         <v>16460616.0161408</v>
       </c>
       <c r="G30" t="s">
@@ -1503,7 +1506,7 @@
       <c r="E31" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="3">
         <v>16855706.995112699</v>
       </c>
       <c r="G31" t="s">
@@ -1532,7 +1535,7 @@
       <c r="E32" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
         <v>17498795.167024501</v>
       </c>
       <c r="G32" t="s">
@@ -1561,7 +1564,7 @@
       <c r="E33" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
         <v>19433026.916823398</v>
       </c>
       <c r="G33" t="s">
@@ -1590,7 +1593,7 @@
       <c r="E34" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="3">
         <v>17414430.917273998</v>
       </c>
       <c r="G34" t="s">
@@ -1619,7 +1622,7 @@
       <c r="E35" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="3">
         <v>17990328.409190599</v>
       </c>
       <c r="G35" t="s">
@@ -1648,7 +1651,7 @@
       <c r="E36" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="3">
         <v>18677591.2983054</v>
       </c>
       <c r="G36" t="s">
@@ -1677,7 +1680,7 @@
       <c r="E37" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="3">
         <v>20777530.458721898</v>
       </c>
       <c r="G37" t="s">
@@ -1706,7 +1709,7 @@
       <c r="E38" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="3">
         <v>18181889.788757</v>
       </c>
       <c r="G38" t="s">
@@ -1735,7 +1738,7 @@
       <c r="E39" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="3">
         <v>18425948.870557599</v>
       </c>
       <c r="G39" t="s">
@@ -1764,7 +1767,7 @@
       <c r="E40" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="3">
         <v>18709673.820023701</v>
       </c>
       <c r="G40" t="s">
@@ -1793,7 +1796,7 @@
       <c r="E41" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="3">
         <v>20359098.9753973</v>
       </c>
       <c r="G41" t="s">
@@ -1822,7 +1825,7 @@
       <c r="E42" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="3">
         <v>18184930.527799699</v>
       </c>
       <c r="G42" t="s">
@@ -1851,7 +1854,7 @@
       <c r="E43" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="3">
         <v>18793111.313244101</v>
       </c>
       <c r="G43" t="s">
@@ -1880,7 +1883,7 @@
       <c r="E44" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="3">
         <v>19572312.623723801</v>
       </c>
       <c r="G44" t="s">
@@ -1909,7 +1912,7 @@
       <c r="E45" t="s">
         <v>18</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="3">
         <v>22175371.678746499</v>
       </c>
       <c r="G45" t="s">
@@ -1938,7 +1941,7 @@
       <c r="E46" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="3">
         <v>19701481.146581098</v>
       </c>
       <c r="G46" t="s">
@@ -1967,7 +1970,7 @@
       <c r="E47" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="3">
         <v>20583918.707255598</v>
       </c>
       <c r="G47" t="s">
@@ -1996,7 +1999,7 @@
       <c r="E48" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="3">
         <v>21361932.1803349</v>
       </c>
       <c r="G48" t="s">
@@ -2025,7 +2028,7 @@
       <c r="E49" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="3">
         <v>23755498.525800802</v>
       </c>
       <c r="G49" t="s">
@@ -2054,7 +2057,7 @@
       <c r="E50" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="3">
         <v>21097535.265048798</v>
       </c>
       <c r="G50" t="s">
@@ -2083,7 +2086,7 @@
       <c r="E51" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="3">
         <v>21753840.250449099</v>
       </c>
       <c r="G51" t="s">
@@ -2112,7 +2115,7 @@
       <c r="E52" t="s">
         <v>17</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="3">
         <v>22538013.4960186</v>
       </c>
       <c r="G52" t="s">
@@ -2141,7 +2144,7 @@
       <c r="E53" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="3">
         <v>24952468.2484328</v>
       </c>
       <c r="G53" t="s">
@@ -2170,7 +2173,7 @@
       <c r="E54" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="3">
         <v>22232256.723938201</v>
       </c>
       <c r="G54" t="s">
@@ -2199,7 +2202,7 @@
       <c r="E55" t="s">
         <v>16</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="3">
         <v>23313979.744098902</v>
       </c>
       <c r="G55" t="s">
@@ -2228,7 +2231,7 @@
       <c r="E56" t="s">
         <v>17</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="3">
         <v>24369093.346130099</v>
       </c>
       <c r="G56" t="s">
@@ -2257,7 +2260,7 @@
       <c r="E57" t="s">
         <v>18</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="3">
         <v>26941292.020383701</v>
       </c>
       <c r="G57" t="s">
@@ -2286,7 +2289,7 @@
       <c r="E58" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="3">
         <v>23411662.736803401</v>
       </c>
       <c r="G58" t="s">
@@ -2315,7 +2318,7 @@
       <c r="E59" t="s">
         <v>16</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59" s="3">
         <v>24463511.795754701</v>
       </c>
       <c r="G59" t="s">
@@ -2344,7 +2347,7 @@
       <c r="E60" t="s">
         <v>17</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="3">
         <v>25293839.963785902</v>
       </c>
       <c r="G60" t="s">
@@ -2373,7 +2376,7 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61" s="3">
         <v>27780831.615456901</v>
       </c>
       <c r="G61" t="s">
@@ -2402,7 +2405,7 @@
       <c r="E62" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="3">
         <v>24251724.782768399</v>
       </c>
       <c r="G62" t="s">
@@ -2431,7 +2434,7 @@
       <c r="E63" t="s">
         <v>16</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="3">
         <v>24364087.6855569</v>
       </c>
       <c r="G63" t="s">
@@ -2460,7 +2463,7 @@
       <c r="E64" t="s">
         <v>17</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="3">
         <v>25156152.161914401</v>
       </c>
       <c r="G64" t="s">
@@ -2489,7 +2492,7 @@
       <c r="E65" t="s">
         <v>18</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="3">
         <v>27298710.036389198</v>
       </c>
       <c r="G65" t="s">
@@ -2518,7 +2521,7 @@
       <c r="E66" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="3">
         <v>23282571.9648881</v>
       </c>
       <c r="G66" t="s">
@@ -2547,7 +2550,7 @@
       <c r="E67" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="3">
         <v>24272826.0578393</v>
       </c>
       <c r="G67" t="s">
@@ -2576,7 +2579,7 @@
       <c r="E68" t="s">
         <v>17</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="3">
         <v>24617172.825777899</v>
       </c>
       <c r="G68" t="s">
@@ -2605,7 +2608,7 @@
       <c r="E69" t="s">
         <v>18</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="3">
         <v>28202783.155630399</v>
       </c>
       <c r="G69" t="s">
@@ -2634,7 +2637,7 @@
       <c r="E70" t="s">
         <v>13</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70" s="3">
         <v>24966378.2597582</v>
       </c>
       <c r="G70" t="s">
@@ -2663,7 +2666,7 @@
       <c r="E71" t="s">
         <v>16</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="3">
         <v>26282121.648133501</v>
       </c>
       <c r="G71" t="s">
@@ -2692,7 +2695,7 @@
       <c r="E72" t="s">
         <v>17</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="3">
         <v>26026696.769151699</v>
       </c>
       <c r="G72" t="s">
@@ -2721,7 +2724,7 @@
       <c r="E73" t="s">
         <v>18</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="3">
         <v>29092967.438434701</v>
       </c>
       <c r="G73" t="s">
@@ -2750,7 +2753,7 @@
       <c r="E74" t="s">
         <v>13</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74" s="3">
         <v>25251450.8924063</v>
       </c>
       <c r="G74" t="s">
@@ -2779,7 +2782,7 @@
       <c r="E75" t="s">
         <v>16</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F75" s="3">
         <v>26416798.848399099</v>
       </c>
       <c r="G75" t="s">
@@ -2808,7 +2811,7 @@
       <c r="E76" t="s">
         <v>17</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76" s="3">
         <v>26612319.2614264</v>
       </c>
       <c r="G76" t="s">
@@ -2837,7 +2840,7 @@
       <c r="E77" t="s">
         <v>18</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77" s="3">
         <v>29198391.997768302</v>
       </c>
       <c r="G77" t="s">
@@ -2866,7 +2869,7 @@
       <c r="E78" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78" s="3">
         <v>25195116.035096198</v>
       </c>
       <c r="G78" t="s">
@@ -2895,7 +2898,7 @@
       <c r="E79" t="s">
         <v>16</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="3">
         <v>26520565.919128101</v>
       </c>
       <c r="G79" t="s">
@@ -2924,7 +2927,7 @@
       <c r="E80" t="s">
         <v>17</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F80" s="3">
         <v>26709303.113683701</v>
       </c>
       <c r="G80" t="s">
@@ -2953,7 +2956,7 @@
       <c r="E81" t="s">
         <v>18</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F81" s="3">
         <v>29231750.9320921</v>
       </c>
       <c r="G81" t="s">
@@ -2982,7 +2985,7 @@
       <c r="E82" t="s">
         <v>13</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82" s="3">
         <v>25297756.124764301</v>
       </c>
       <c r="G82" t="s">
@@ -3011,7 +3014,7 @@
       <c r="E83" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83" s="3">
         <v>21335355.067193698</v>
       </c>
       <c r="G83" t="s">
@@ -3040,7 +3043,7 @@
       <c r="E84" t="s">
         <v>17</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F84" s="3">
         <v>23764364.515104599</v>
       </c>
       <c r="G84" t="s">
@@ -3069,7 +3072,7 @@
       <c r="E85" t="s">
         <v>18</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F85" s="3">
         <v>27306291.474640299</v>
       </c>
       <c r="G85" t="s">
@@ -3098,7 +3101,7 @@
       <c r="E86" t="s">
         <v>13</v>
       </c>
-      <c r="F86" s="2">
+      <c r="F86" s="3">
         <v>23965888.540973399</v>
       </c>
       <c r="G86" t="s">
@@ -3127,7 +3130,7 @@
       <c r="E87" t="s">
         <v>16</v>
       </c>
-      <c r="F87" s="2">
+      <c r="F87" s="3">
         <v>26091223.144167699</v>
       </c>
       <c r="G87" t="s">
@@ -3156,7 +3159,7 @@
       <c r="E88" t="s">
         <v>17</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F88" s="3">
         <v>26970736.706119701</v>
       </c>
       <c r="G88" t="s">
@@ -3185,7 +3188,7 @@
       <c r="E89" t="s">
         <v>18</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F89" s="3">
         <v>30268882.180841599</v>
       </c>
       <c r="G89" t="s">
@@ -3214,7 +3217,7 @@
       <c r="E90" t="s">
         <v>13</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F90" s="3">
         <v>26469576.131496198</v>
       </c>
       <c r="G90" t="s">
@@ -3243,7 +3246,7 @@
       <c r="E91" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91" s="3">
         <v>27624457.7588205</v>
       </c>
       <c r="G91" t="s">
@@ -3272,7 +3275,7 @@
       <c r="E92" t="s">
         <v>17</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F92" s="3">
         <v>28796599.0097946</v>
       </c>
       <c r="G92" t="s">
@@ -3301,7 +3304,7 @@
       <c r="E93" t="s">
         <v>18</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F93" s="3">
         <v>31043622.946359299</v>
       </c>
       <c r="G93" t="s">
@@ -3330,7 +3333,7 @@
       <c r="E94" t="s">
         <v>13</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F94" s="3">
         <v>27827214.3242217</v>
       </c>
       <c r="G94" t="s">
@@ -3359,7 +3362,7 @@
       <c r="E95" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95" s="3">
         <v>28967281.591732401</v>
       </c>
       <c r="G95" t="s">
@@ -3388,7 +3391,7 @@
       <c r="E96" t="s">
         <v>17</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F96" s="3">
         <v>28903945.8360782</v>
       </c>
       <c r="G96" t="s">
@@ -3430,7 +3433,7 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>311</v>
       </c>
     </row>
@@ -3504,7 +3507,7 @@
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>